<commit_message>
Actualizacion forma de pago
</commit_message>
<xml_diff>
--- a/uploads/movimientos.xlsx
+++ b/uploads/movimientos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0A37C8-212F-4242-88E1-E612188FEAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D37FFB-0B59-48F4-B5C2-CF0012E44648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Movimientos de Cuenta</t>
   </si>
@@ -75,6 +75,57 @@
   </si>
   <si>
     <t>306949090</t>
+  </si>
+  <si>
+    <t>2025-10-13, 5:44 PM</t>
+  </si>
+  <si>
+    <t>$353,18</t>
+  </si>
+  <si>
+    <t>306866418</t>
+  </si>
+  <si>
+    <t>2025-10-13, 3:30 PM</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DIRECTA DE QUEVEDO AIZPRUA ANTHONY FERNANDO</t>
+  </si>
+  <si>
+    <t>$333,18</t>
+  </si>
+  <si>
+    <t>292651038</t>
+  </si>
+  <si>
+    <t>2025-10-13, 1:38 PM</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DIRECTA A LARA  MALDONADO LUIS ALBERTO</t>
+  </si>
+  <si>
+    <t>Débito</t>
+  </si>
+  <si>
+    <t>-$20,00</t>
+  </si>
+  <si>
+    <t>$313,18</t>
+  </si>
+  <si>
+    <t>279762674</t>
+  </si>
+  <si>
+    <t>2025-10-13, 1:37 PM</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DIRECTA A MORA  MARCILLO AMANDO</t>
+  </si>
+  <si>
+    <t>-$30,00</t>
+  </si>
+  <si>
+    <t>279634470</t>
   </si>
 </sst>
 </file>
@@ -372,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -419,6 +470,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:R407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1043,7 +1098,7 @@
       <c r="N12" s="14"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="15"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="1.05" customHeight="1">
@@ -1090,19 +1145,29 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="F15" s="12"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="L15" s="13"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="12"/>
+      <c r="O15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
@@ -1114,7 +1179,9 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="14"/>
+      <c r="H16" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="13"/>
@@ -1170,19 +1237,29 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="F19" s="12"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="13"/>
+      <c r="K19" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="L19" s="13"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="12"/>
+      <c r="O19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
@@ -1194,7 +1271,9 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="13"/>
@@ -1250,19 +1329,29 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="D23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F23" s="12"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="12"/>
+      <c r="K23" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="L23" s="12"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
+      <c r="O23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
@@ -1274,7 +1363,9 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="12"/>
@@ -1330,19 +1421,29 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="D27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="F27" s="12"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="12"/>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="L27" s="12"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
+      <c r="O27" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
@@ -1354,7 +1455,9 @@
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="12"/>

</xml_diff>